<commit_message>
created reallocate.py, added catValuesList function to main_functions.py
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -211,7 +211,10 @@
     <t xml:space="preserve">Max_Taxed_Sales</t>
   </si>
   <si>
-    <t xml:space="preserve">Needed IRA Contribution</t>
+    <t xml:space="preserve">Needed Qualified Contribution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HSA min</t>
   </si>
   <si>
     <t xml:space="preserve">Tax Status</t>
@@ -583,16 +586,16 @@
   </sheetPr>
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="18" min="1" style="0" width="16.3316326530612"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="18" min="1" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1484,13 +1487,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="35.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1729,13 +1732,14 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1763,8 +1767,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="16"/>
-      <c r="B4" s="8"/>
+      <c r="A4" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="8" t="n">
+        <v>5000</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="16"/>
@@ -1798,12 +1806,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1811,13 +1821,13 @@
         <v>3</v>
       </c>
       <c r="B1" s="22" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1825,41 +1835,41 @@
         <v>40</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="24" t="s">
         <v>69</v>
-      </c>
-      <c r="B3" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="D3" s="24" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,111 +1877,111 @@
         <v>29</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="23" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B7" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B8" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="23" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1979,13 +1989,13 @@
         <v>25</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1993,13 +2003,13 @@
         <v>23</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2007,27 +2017,27 @@
         <v>50</v>
       </c>
       <c r="B15" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B16" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>82</v>
-      </c>
       <c r="D16" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2035,100 +2045,100 @@
         <v>53</v>
       </c>
       <c r="B17" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F17" s="25"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="23" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B18" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F18" s="25"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B19" s="24" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F19" s="25"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B20" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="23" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D21" s="24" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D22" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2136,41 +2146,41 @@
         <v>35</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
FundingRequest class, test_funding_request, create fundingRequestList in initialize_objects
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Desired_Allocation" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Other_inputs" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Tax_Status" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Fund_Accounts" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="96">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -302,6 +303,15 @@
   </si>
   <si>
     <t xml:space="preserve">Ltd Ptnr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Funding Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Account to Fund</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amount to Fund</t>
   </si>
 </sst>
 </file>
@@ -458,7 +468,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,6 +575,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -587,17 +601,16 @@
   <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+      <selection pane="topLeft" activeCell="Q22" activeCellId="0" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="19.0357142857143"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.3265306122449"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1489,13 +1502,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.4234693877551"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.17857142857143"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1734,13 +1745,14 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1798,17 +1810,19 @@
   <dimension ref="A1:F65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="28.6173469387755"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2188,4 +2202,89 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>9999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
funding requests now considers min cash rules
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" state="visible" r:id="rId2"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="105">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -628,8 +628,8 @@
   </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2301,7 +2301,7 @@
   </sheetPr>
   <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
@@ -2424,21 +2424,21 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E29" activeCellId="0" sqref="E29"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4897959183673"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2959183673469"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1275510204082"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2446,18 +2446,21 @@
         <v>0</v>
       </c>
       <c r="B1" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="27" t="s">
         <v>99</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="D1" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D1" s="27" t="s">
+      <c r="E1" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="E1" s="27" t="s">
+      <c r="F1" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="G1" s="13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2465,13 +2468,16 @@
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="8" t="n">
+      <c r="B2" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="8" t="n">
         <v>5000</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="8" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="8" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2479,79 +2485,90 @@
       <c r="A3" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="B3" s="8"/>
-      <c r="C3" s="20" t="n">
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="20" t="n">
         <v>0.03</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="8"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="20"/>
+      <c r="G4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="20"/>
+      <c r="G7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="20"/>
+      <c r="G9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="8"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="20"/>
+      <c r="G11" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
excel tab Category_Rules added
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,6 +14,7 @@
     <sheet name="Tax_Status" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Fund_Accounts" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Account_Min_Max" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="Category_Rules" sheetId="7" state="visible" r:id="rId8"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="111">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -340,6 +341,24 @@
   </si>
   <si>
     <t xml:space="preserve">HSA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Count As</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sell First</t>
   </si>
 </sst>
 </file>
@@ -628,17 +647,18 @@
   </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="18" min="5" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="21.0612244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="21" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="18.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1592,11 +1612,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.719387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="36.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1841,8 +1863,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.8928571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.4897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1905,14 +1927,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.8061224489796"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2307,10 +2329,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.3571428571429"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5969387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2432,13 +2453,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.9336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.7397959183673"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.4897959183673"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.2959183673469"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.1275510204082"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2569,6 +2590,171 @@
       <c r="E11" s="8"/>
       <c r="F11" s="20"/>
       <c r="G11" s="8"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="20"/>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="8"/>
+      <c r="E4" s="20"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="20" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="20" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="20"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="20"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="20"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="20"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="20"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="20"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="20"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
initilized category rules dictionary and modification of Category_Rules tab
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="112">
   <si>
     <t xml:space="preserve">Account</t>
   </si>
@@ -349,13 +349,16 @@
     <t xml:space="preserve">Rule</t>
   </si>
   <si>
+    <t xml:space="preserve">Count As Category</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed</t>
+  </si>
+  <si>
     <t xml:space="preserve">Count As</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Percent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fixed</t>
   </si>
   <si>
     <t xml:space="preserve">Sell First</t>
@@ -2610,13 +2613,16 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+      <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2656,7 +2662,9 @@
       <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="D3" s="8" t="s">
         <v>15</v>
       </c>
@@ -2672,7 +2680,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="D4" s="8"/>
       <c r="E4" s="20"/>
@@ -2684,7 +2692,9 @@
       <c r="B5" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="D5" s="8" t="s">
         <v>5</v>
       </c>
@@ -2699,7 +2709,9 @@
       <c r="B6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="8" t="s">
+        <v>110</v>
+      </c>
       <c r="D6" s="8" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
start of unit testing, sellFirstCategories function
</commit_message>
<xml_diff>
--- a/Allocation_Template.xlsx
+++ b/Allocation_Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Accounts" sheetId="1" state="visible" r:id="rId2"/>
@@ -650,8 +650,8 @@
   </sheetPr>
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="R15" activeCellId="0" sqref="R15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2612,7 +2612,7 @@
   </sheetPr>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
     </sheetView>
   </sheetViews>

</xml_diff>